<commit_message>
Petites corrections index et essais CSS
</commit_message>
<xml_diff>
--- a/FichierCompletBaseANONYME.xlsx
+++ b/FichierCompletBaseANONYME.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gut/Documents/Université/MASTER/TRAVAIL MASTER/Tableaux Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gut/Documents/GitHub/VisuDo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66D3A50-D635-464B-A82D-824038EF5696}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E37CE66-88DA-A846-A342-957C3F0C9634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35420" windowHeight="21900" xr2:uid="{2AD2CF4C-7C03-1D42-B68B-D7D67D183A68}"/>
   </bookViews>
@@ -1334,7 +1334,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C79" sqref="C79"/>
+      <selection pane="topRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4853,7 +4853,9 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="K17" s="2">
+        <v>2</v>
+      </c>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" t="s">
@@ -7069,7 +7071,9 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
+      <c r="K28" s="2">
+        <v>2</v>
+      </c>
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
       <c r="N28" t="s">
@@ -7923,7 +7927,9 @@
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
+      <c r="K32" s="2">
+        <v>2</v>
+      </c>
       <c r="L32" s="2"/>
       <c r="M32" s="2"/>
       <c r="N32" t="s">
@@ -12743,7 +12749,9 @@
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
       <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
+      <c r="K54" s="6">
+        <v>3</v>
+      </c>
       <c r="L54" s="6"/>
       <c r="M54" s="6"/>
       <c r="N54" t="s">
@@ -13429,7 +13437,9 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
+      <c r="K57" s="6">
+        <v>1</v>
+      </c>
       <c r="L57" s="6"/>
       <c r="M57" s="6"/>
       <c r="N57" t="s">
@@ -15505,7 +15515,7 @@
         <v>1993</v>
       </c>
       <c r="E66" s="13">
-        <f t="shared" ref="E66:E97" si="2">2021 - D66</f>
+        <f t="shared" ref="E66:E78" si="2">2021 - D66</f>
         <v>28</v>
       </c>
       <c r="F66" s="6">
@@ -16005,7 +16015,9 @@
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
-      <c r="K68" s="6"/>
+      <c r="K68" s="6">
+        <v>4</v>
+      </c>
       <c r="L68" s="6"/>
       <c r="M68" s="6"/>
       <c r="N68" t="s">
@@ -16445,7 +16457,9 @@
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
       <c r="J70" s="6"/>
-      <c r="K70" s="6"/>
+      <c r="K70" s="6">
+        <v>3</v>
+      </c>
       <c r="L70" s="6"/>
       <c r="M70" s="6"/>
       <c r="N70" t="s">
@@ -17377,7 +17391,9 @@
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
       <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
+      <c r="K74" s="6">
+        <v>4</v>
+      </c>
       <c r="L74" s="6"/>
       <c r="M74" s="6"/>
       <c r="N74" t="s">
@@ -17571,7 +17587,9 @@
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
       <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
+      <c r="K75" s="6">
+        <v>3</v>
+      </c>
       <c r="L75" s="6"/>
       <c r="M75" s="6"/>
       <c r="N75" t="s">
@@ -17765,7 +17783,9 @@
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
-      <c r="K76" s="6"/>
+      <c r="K76" s="6">
+        <v>4</v>
+      </c>
       <c r="L76" s="6"/>
       <c r="M76" s="6"/>
       <c r="N76" t="s">

</xml_diff>